<commit_message>
Created script to modify text file using the flight mission cycle
</commit_message>
<xml_diff>
--- a/Generating Flight Mission Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating Flight Mission Cycle/Flight_Mission_Cycle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating Flight Mission Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DE1262F-E268-4F67-80B2-D42BB392F9D8}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,26 +821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1075,26 +1055,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1111,4 +1092,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>